<commit_message>
made changes to reg
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/register_openCart.xlsx
+++ b/src/test/resources/testdata/register_openCart.xlsx
@@ -1,21 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECEF45CA-1054-4B16-B673-6FCA52D71EF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{0D89F48B-A4CF-413A-9861-296E954F688E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{BD526D63-9046-49D1-9E28-49D108F039A4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BD526D63-9046-49D1-9E28-49D108F039A4}"/>
   </bookViews>
   <sheets>
     <sheet name="register" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>firstname</t>
   </si>
@@ -42,39 +38,18 @@
     <t>subscribe</t>
   </si>
   <si>
-    <t>kiyaan</t>
-  </si>
-  <si>
-    <t>khalde</t>
-  </si>
-  <si>
     <t>123@test</t>
   </si>
   <si>
     <t>yes</t>
   </si>
   <si>
-    <t>ira</t>
-  </si>
-  <si>
-    <t>kanse</t>
-  </si>
-  <si>
     <t>ira@34</t>
   </si>
   <si>
     <t>no</t>
   </si>
   <si>
-    <t>aabha</t>
-  </si>
-  <si>
-    <t>aabha34</t>
-  </si>
-  <si>
-    <t>somwanshi</t>
-  </si>
-  <si>
     <t>9267899098</t>
   </si>
   <si>
@@ -82,6 +57,21 @@
   </si>
   <si>
     <t>9898765432</t>
+  </si>
+  <si>
+    <t>amir</t>
+  </si>
+  <si>
+    <t>iravati</t>
+  </si>
+  <si>
+    <t>anu</t>
+  </si>
+  <si>
+    <t>tester</t>
+  </si>
+  <si>
+    <t>anu34</t>
   </si>
 </sst>
 </file>
@@ -470,19 +460,19 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -499,55 +489,55 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>